<commit_message>
convert time second to minute
</commit_message>
<xml_diff>
--- a/backend/imag_commplc-mysql/src/main/resources/DataExcel/Data.xlsx
+++ b/backend/imag_commplc-mysql/src/main/resources/DataExcel/Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216493" uniqueCount="3979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3232273" uniqueCount="3999">
   <si>
     <t>Line</t>
   </si>
@@ -11971,6 +11971,66 @@
   </si>
   <si>
     <t>1856</t>
+  </si>
+  <si>
+    <t>6176</t>
+  </si>
+  <si>
+    <t>6177</t>
+  </si>
+  <si>
+    <t>6178</t>
+  </si>
+  <si>
+    <t>6179</t>
+  </si>
+  <si>
+    <t>6180</t>
+  </si>
+  <si>
+    <t>6181</t>
+  </si>
+  <si>
+    <t>6182</t>
+  </si>
+  <si>
+    <t>6183</t>
+  </si>
+  <si>
+    <t>6184</t>
+  </si>
+  <si>
+    <t>6185</t>
+  </si>
+  <si>
+    <t>6186</t>
+  </si>
+  <si>
+    <t>6187</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>513</t>
+  </si>
+  <si>
+    <t>514</t>
+  </si>
+  <si>
+    <t>519</t>
+  </si>
+  <si>
+    <t>520</t>
+  </si>
+  <si>
+    <t>521</t>
+  </si>
+  <si>
+    <t>522</t>
   </si>
 </sst>
 </file>
@@ -12352,7 +12412,7 @@
         <v>6000</v>
       </c>
       <c r="D2" t="s">
-        <v>255</v>
+        <v>3856</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -12361,7 +12421,7 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>258</v>
+        <v>3991</v>
       </c>
       <c r="H2">
         <v>25</v>
@@ -12406,7 +12466,7 @@
         <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>3992</v>
       </c>
       <c r="H3">
         <v>37</v>
@@ -12451,7 +12511,7 @@
         <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>3992</v>
       </c>
       <c r="H4">
         <v>51</v>
@@ -12496,7 +12556,7 @@
         <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>3992</v>
       </c>
       <c r="H5">
         <v>51</v>
@@ -12541,7 +12601,7 @@
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>3992</v>
       </c>
       <c r="H6">
         <v>51</v>
@@ -12586,7 +12646,7 @@
         <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>3992</v>
       </c>
       <c r="H7">
         <v>51</v>
@@ -12631,7 +12691,7 @@
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>3992</v>
       </c>
       <c r="H8">
         <v>51</v>
@@ -12676,7 +12736,7 @@
         <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>3992</v>
       </c>
       <c r="H9">
         <v>51</v>
@@ -12721,7 +12781,7 @@
         <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>3992</v>
       </c>
       <c r="H10">
         <v>51</v>
@@ -12766,7 +12826,7 @@
         <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>3992</v>
       </c>
       <c r="H11">
         <v>51</v>
@@ -12811,7 +12871,7 @@
         <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>3992</v>
       </c>
       <c r="H12">
         <v>51</v>
@@ -12856,7 +12916,7 @@
         <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>3992</v>
       </c>
       <c r="H13">
         <v>51</v>

</xml_diff>

<commit_message>
add reconnect plc feature, add API filter
</commit_message>
<xml_diff>
--- a/backend/imag_commplc-mysql/src/main/resources/DataExcel/Data.xlsx
+++ b/backend/imag_commplc-mysql/src/main/resources/DataExcel/Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376873" uniqueCount="4203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498673" uniqueCount="4818">
   <si>
     <t>Line</t>
   </si>
@@ -12643,6 +12643,1851 @@
   </si>
   <si>
     <t>22.0</t>
+  </si>
+  <si>
+    <t>5080</t>
+  </si>
+  <si>
+    <t>97.0</t>
+  </si>
+  <si>
+    <t>5082</t>
+  </si>
+  <si>
+    <t>5083</t>
+  </si>
+  <si>
+    <t>5084</t>
+  </si>
+  <si>
+    <t>5085</t>
+  </si>
+  <si>
+    <t>5086</t>
+  </si>
+  <si>
+    <t>5087</t>
+  </si>
+  <si>
+    <t>5088</t>
+  </si>
+  <si>
+    <t>5089</t>
+  </si>
+  <si>
+    <t>5090</t>
+  </si>
+  <si>
+    <t>5091</t>
+  </si>
+  <si>
+    <t>5092</t>
+  </si>
+  <si>
+    <t>5139</t>
+  </si>
+  <si>
+    <t>5140</t>
+  </si>
+  <si>
+    <t>5141</t>
+  </si>
+  <si>
+    <t>5142</t>
+  </si>
+  <si>
+    <t>5143</t>
+  </si>
+  <si>
+    <t>5144</t>
+  </si>
+  <si>
+    <t>5145</t>
+  </si>
+  <si>
+    <t>98.0</t>
+  </si>
+  <si>
+    <t>5146</t>
+  </si>
+  <si>
+    <t>5147</t>
+  </si>
+  <si>
+    <t>5148</t>
+  </si>
+  <si>
+    <t>5149</t>
+  </si>
+  <si>
+    <t>5150</t>
+  </si>
+  <si>
+    <t>5151</t>
+  </si>
+  <si>
+    <t>5152</t>
+  </si>
+  <si>
+    <t>5153</t>
+  </si>
+  <si>
+    <t>5338</t>
+  </si>
+  <si>
+    <t>5339</t>
+  </si>
+  <si>
+    <t>5340</t>
+  </si>
+  <si>
+    <t>5341</t>
+  </si>
+  <si>
+    <t>5342</t>
+  </si>
+  <si>
+    <t>5343</t>
+  </si>
+  <si>
+    <t>5344</t>
+  </si>
+  <si>
+    <t>5345</t>
+  </si>
+  <si>
+    <t>5346</t>
+  </si>
+  <si>
+    <t>5347</t>
+  </si>
+  <si>
+    <t>5564</t>
+  </si>
+  <si>
+    <t>103.0</t>
+  </si>
+  <si>
+    <t>5566</t>
+  </si>
+  <si>
+    <t>5567</t>
+  </si>
+  <si>
+    <t>5568</t>
+  </si>
+  <si>
+    <t>5569</t>
+  </si>
+  <si>
+    <t>5570</t>
+  </si>
+  <si>
+    <t>5611</t>
+  </si>
+  <si>
+    <t>104.0</t>
+  </si>
+  <si>
+    <t>5612</t>
+  </si>
+  <si>
+    <t>5613</t>
+  </si>
+  <si>
+    <t>5614</t>
+  </si>
+  <si>
+    <t>5615</t>
+  </si>
+  <si>
+    <t>5616</t>
+  </si>
+  <si>
+    <t>5617</t>
+  </si>
+  <si>
+    <t>5618</t>
+  </si>
+  <si>
+    <t>5619</t>
+  </si>
+  <si>
+    <t>5620</t>
+  </si>
+  <si>
+    <t>5621</t>
+  </si>
+  <si>
+    <t>5622</t>
+  </si>
+  <si>
+    <t>5623</t>
+  </si>
+  <si>
+    <t>5624</t>
+  </si>
+  <si>
+    <t>5654</t>
+  </si>
+  <si>
+    <t>105.0</t>
+  </si>
+  <si>
+    <t>5655</t>
+  </si>
+  <si>
+    <t>5656</t>
+  </si>
+  <si>
+    <t>5657</t>
+  </si>
+  <si>
+    <t>106.0</t>
+  </si>
+  <si>
+    <t>5972</t>
+  </si>
+  <si>
+    <t>109.0</t>
+  </si>
+  <si>
+    <t>5973</t>
+  </si>
+  <si>
+    <t>6451</t>
+  </si>
+  <si>
+    <t>116.0</t>
+  </si>
+  <si>
+    <t>6452</t>
+  </si>
+  <si>
+    <t>6453</t>
+  </si>
+  <si>
+    <t>6454</t>
+  </si>
+  <si>
+    <t>6455</t>
+  </si>
+  <si>
+    <t>6456</t>
+  </si>
+  <si>
+    <t>6524</t>
+  </si>
+  <si>
+    <t>117.0</t>
+  </si>
+  <si>
+    <t>6556</t>
+  </si>
+  <si>
+    <t>6557</t>
+  </si>
+  <si>
+    <t>6558</t>
+  </si>
+  <si>
+    <t>6559</t>
+  </si>
+  <si>
+    <t>6560</t>
+  </si>
+  <si>
+    <t>6567</t>
+  </si>
+  <si>
+    <t>6568</t>
+  </si>
+  <si>
+    <t>6569</t>
+  </si>
+  <si>
+    <t>6572</t>
+  </si>
+  <si>
+    <t>6573</t>
+  </si>
+  <si>
+    <t>6574</t>
+  </si>
+  <si>
+    <t>6575</t>
+  </si>
+  <si>
+    <t>6576</t>
+  </si>
+  <si>
+    <t>6577</t>
+  </si>
+  <si>
+    <t>11378</t>
+  </si>
+  <si>
+    <t>184.0</t>
+  </si>
+  <si>
+    <t>11379</t>
+  </si>
+  <si>
+    <t>11380</t>
+  </si>
+  <si>
+    <t>11381</t>
+  </si>
+  <si>
+    <t>11382</t>
+  </si>
+  <si>
+    <t>11383</t>
+  </si>
+  <si>
+    <t>11822</t>
+  </si>
+  <si>
+    <t>11823</t>
+  </si>
+  <si>
+    <t>11824</t>
+  </si>
+  <si>
+    <t>11825</t>
+  </si>
+  <si>
+    <t>11826</t>
+  </si>
+  <si>
+    <t>11827</t>
+  </si>
+  <si>
+    <t>11828</t>
+  </si>
+  <si>
+    <t>11876</t>
+  </si>
+  <si>
+    <t>11877</t>
+  </si>
+  <si>
+    <t>11878</t>
+  </si>
+  <si>
+    <t>11879</t>
+  </si>
+  <si>
+    <t>11880</t>
+  </si>
+  <si>
+    <t>11902</t>
+  </si>
+  <si>
+    <t>11903</t>
+  </si>
+  <si>
+    <t>11904</t>
+  </si>
+  <si>
+    <t>11905</t>
+  </si>
+  <si>
+    <t>11906</t>
+  </si>
+  <si>
+    <t>12008</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>12009</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>12010</t>
+  </si>
+  <si>
+    <t>12011</t>
+  </si>
+  <si>
+    <t>12012</t>
+  </si>
+  <si>
+    <t>12013</t>
+  </si>
+  <si>
+    <t>12014</t>
+  </si>
+  <si>
+    <t>12015</t>
+  </si>
+  <si>
+    <t>12016</t>
+  </si>
+  <si>
+    <t>12017</t>
+  </si>
+  <si>
+    <t>12018</t>
+  </si>
+  <si>
+    <t>12019</t>
+  </si>
+  <si>
+    <t>12020</t>
+  </si>
+  <si>
+    <t>12021</t>
+  </si>
+  <si>
+    <t>12022</t>
+  </si>
+  <si>
+    <t>12023</t>
+  </si>
+  <si>
+    <t>12024</t>
+  </si>
+  <si>
+    <t>12025</t>
+  </si>
+  <si>
+    <t>12026</t>
+  </si>
+  <si>
+    <t>12027</t>
+  </si>
+  <si>
+    <t>12028</t>
+  </si>
+  <si>
+    <t>12029</t>
+  </si>
+  <si>
+    <t>12030</t>
+  </si>
+  <si>
+    <t>12031</t>
+  </si>
+  <si>
+    <t>12032</t>
+  </si>
+  <si>
+    <t>12033</t>
+  </si>
+  <si>
+    <t>12034</t>
+  </si>
+  <si>
+    <t>12035</t>
+  </si>
+  <si>
+    <t>12036</t>
+  </si>
+  <si>
+    <t>12037</t>
+  </si>
+  <si>
+    <t>12038</t>
+  </si>
+  <si>
+    <t>12039</t>
+  </si>
+  <si>
+    <t>12040</t>
+  </si>
+  <si>
+    <t>12041</t>
+  </si>
+  <si>
+    <t>12042</t>
+  </si>
+  <si>
+    <t>12043</t>
+  </si>
+  <si>
+    <t>12044</t>
+  </si>
+  <si>
+    <t>12045</t>
+  </si>
+  <si>
+    <t>67.0</t>
+  </si>
+  <si>
+    <t>12046</t>
+  </si>
+  <si>
+    <t>12047</t>
+  </si>
+  <si>
+    <t>12048</t>
+  </si>
+  <si>
+    <t>12049</t>
+  </si>
+  <si>
+    <t>12050</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>12051</t>
+  </si>
+  <si>
+    <t>51.0</t>
+  </si>
+  <si>
+    <t>12052</t>
+  </si>
+  <si>
+    <t>12053</t>
+  </si>
+  <si>
+    <t>12054</t>
+  </si>
+  <si>
+    <t>12055</t>
+  </si>
+  <si>
+    <t>12056</t>
+  </si>
+  <si>
+    <t>12057</t>
+  </si>
+  <si>
+    <t>12058</t>
+  </si>
+  <si>
+    <t>12059</t>
+  </si>
+  <si>
+    <t>12060</t>
+  </si>
+  <si>
+    <t>12061</t>
+  </si>
+  <si>
+    <t>12062</t>
+  </si>
+  <si>
+    <t>12063</t>
+  </si>
+  <si>
+    <t>12064</t>
+  </si>
+  <si>
+    <t>12065</t>
+  </si>
+  <si>
+    <t>12066</t>
+  </si>
+  <si>
+    <t>12067</t>
+  </si>
+  <si>
+    <t>12068</t>
+  </si>
+  <si>
+    <t>3001</t>
+  </si>
+  <si>
+    <t>3002</t>
+  </si>
+  <si>
+    <t>3003</t>
+  </si>
+  <si>
+    <t>3004</t>
+  </si>
+  <si>
+    <t>3005</t>
+  </si>
+  <si>
+    <t>3006</t>
+  </si>
+  <si>
+    <t>3007</t>
+  </si>
+  <si>
+    <t>3008</t>
+  </si>
+  <si>
+    <t>3009</t>
+  </si>
+  <si>
+    <t>3010</t>
+  </si>
+  <si>
+    <t>3011</t>
+  </si>
+  <si>
+    <t>3012</t>
+  </si>
+  <si>
+    <t>3013</t>
+  </si>
+  <si>
+    <t>3014</t>
+  </si>
+  <si>
+    <t>3015</t>
+  </si>
+  <si>
+    <t>3016</t>
+  </si>
+  <si>
+    <t>3017</t>
+  </si>
+  <si>
+    <t>3018</t>
+  </si>
+  <si>
+    <t>3019</t>
+  </si>
+  <si>
+    <t>52.0</t>
+  </si>
+  <si>
+    <t>54.0</t>
+  </si>
+  <si>
+    <t>1239</t>
+  </si>
+  <si>
+    <t>1240</t>
+  </si>
+  <si>
+    <t>1241</t>
+  </si>
+  <si>
+    <t>1242</t>
+  </si>
+  <si>
+    <t>55.0</t>
+  </si>
+  <si>
+    <t>56.0</t>
+  </si>
+  <si>
+    <t>57.0</t>
+  </si>
+  <si>
+    <t>1504</t>
+  </si>
+  <si>
+    <t>58.0</t>
+  </si>
+  <si>
+    <t>1505</t>
+  </si>
+  <si>
+    <t>1506</t>
+  </si>
+  <si>
+    <t>1507</t>
+  </si>
+  <si>
+    <t>59.0</t>
+  </si>
+  <si>
+    <t>1598</t>
+  </si>
+  <si>
+    <t>1599</t>
+  </si>
+  <si>
+    <t>1600</t>
+  </si>
+  <si>
+    <t>1601</t>
+  </si>
+  <si>
+    <t>1602</t>
+  </si>
+  <si>
+    <t>1603</t>
+  </si>
+  <si>
+    <t>1681</t>
+  </si>
+  <si>
+    <t>60.0</t>
+  </si>
+  <si>
+    <t>1682</t>
+  </si>
+  <si>
+    <t>1683</t>
+  </si>
+  <si>
+    <t>61.0</t>
+  </si>
+  <si>
+    <t>1684</t>
+  </si>
+  <si>
+    <t>1685</t>
+  </si>
+  <si>
+    <t>62.0</t>
+  </si>
+  <si>
+    <t>1803</t>
+  </si>
+  <si>
+    <t>1804</t>
+  </si>
+  <si>
+    <t>1805</t>
+  </si>
+  <si>
+    <t>1806</t>
+  </si>
+  <si>
+    <t>1807</t>
+  </si>
+  <si>
+    <t>1808</t>
+  </si>
+  <si>
+    <t>1809</t>
+  </si>
+  <si>
+    <t>1810</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>1812</t>
+  </si>
+  <si>
+    <t>1813</t>
+  </si>
+  <si>
+    <t>1827</t>
+  </si>
+  <si>
+    <t>1828</t>
+  </si>
+  <si>
+    <t>63.0</t>
+  </si>
+  <si>
+    <t>1829</t>
+  </si>
+  <si>
+    <t>1830</t>
+  </si>
+  <si>
+    <t>1831</t>
+  </si>
+  <si>
+    <t>1832</t>
+  </si>
+  <si>
+    <t>1927</t>
+  </si>
+  <si>
+    <t>64.0</t>
+  </si>
+  <si>
+    <t>1928</t>
+  </si>
+  <si>
+    <t>1929</t>
+  </si>
+  <si>
+    <t>1977</t>
+  </si>
+  <si>
+    <t>65.0</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>1979</t>
+  </si>
+  <si>
+    <t>1980</t>
+  </si>
+  <si>
+    <t>1981</t>
+  </si>
+  <si>
+    <t>1983</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>2026</t>
+  </si>
+  <si>
+    <t>2027</t>
+  </si>
+  <si>
+    <t>2028</t>
+  </si>
+  <si>
+    <t>2029</t>
+  </si>
+  <si>
+    <t>2030</t>
+  </si>
+  <si>
+    <t>2031</t>
+  </si>
+  <si>
+    <t>2032</t>
+  </si>
+  <si>
+    <t>2033</t>
+  </si>
+  <si>
+    <t>2034</t>
+  </si>
+  <si>
+    <t>2035</t>
+  </si>
+  <si>
+    <t>2036</t>
+  </si>
+  <si>
+    <t>2037</t>
+  </si>
+  <si>
+    <t>2038</t>
+  </si>
+  <si>
+    <t>2039</t>
+  </si>
+  <si>
+    <t>2040</t>
+  </si>
+  <si>
+    <t>2041</t>
+  </si>
+  <si>
+    <t>2042</t>
+  </si>
+  <si>
+    <t>66.0</t>
+  </si>
+  <si>
+    <t>2043</t>
+  </si>
+  <si>
+    <t>2044</t>
+  </si>
+  <si>
+    <t>2045</t>
+  </si>
+  <si>
+    <t>2046</t>
+  </si>
+  <si>
+    <t>2047</t>
+  </si>
+  <si>
+    <t>2048</t>
+  </si>
+  <si>
+    <t>2049</t>
+  </si>
+  <si>
+    <t>2050</t>
+  </si>
+  <si>
+    <t>2051</t>
+  </si>
+  <si>
+    <t>2052</t>
+  </si>
+  <si>
+    <t>2053</t>
+  </si>
+  <si>
+    <t>2054</t>
+  </si>
+  <si>
+    <t>2055</t>
+  </si>
+  <si>
+    <t>2056</t>
+  </si>
+  <si>
+    <t>2057</t>
+  </si>
+  <si>
+    <t>2058</t>
+  </si>
+  <si>
+    <t>2059</t>
+  </si>
+  <si>
+    <t>2060</t>
+  </si>
+  <si>
+    <t>2061</t>
+  </si>
+  <si>
+    <t>2062</t>
+  </si>
+  <si>
+    <t>2063</t>
+  </si>
+  <si>
+    <t>2064</t>
+  </si>
+  <si>
+    <t>2065</t>
+  </si>
+  <si>
+    <t>2066</t>
+  </si>
+  <si>
+    <t>2067</t>
+  </si>
+  <si>
+    <t>2068</t>
+  </si>
+  <si>
+    <t>2069</t>
+  </si>
+  <si>
+    <t>2070</t>
+  </si>
+  <si>
+    <t>2071</t>
+  </si>
+  <si>
+    <t>2072</t>
+  </si>
+  <si>
+    <t>2074</t>
+  </si>
+  <si>
+    <t>2075</t>
+  </si>
+  <si>
+    <t>2076</t>
+  </si>
+  <si>
+    <t>2077</t>
+  </si>
+  <si>
+    <t>2078</t>
+  </si>
+  <si>
+    <t>2079</t>
+  </si>
+  <si>
+    <t>2080</t>
+  </si>
+  <si>
+    <t>2081</t>
+  </si>
+  <si>
+    <t>2082</t>
+  </si>
+  <si>
+    <t>2083</t>
+  </si>
+  <si>
+    <t>2084</t>
+  </si>
+  <si>
+    <t>2085</t>
+  </si>
+  <si>
+    <t>2086</t>
+  </si>
+  <si>
+    <t>2087</t>
+  </si>
+  <si>
+    <t>2088</t>
+  </si>
+  <si>
+    <t>2089</t>
+  </si>
+  <si>
+    <t>2090</t>
+  </si>
+  <si>
+    <t>2091</t>
+  </si>
+  <si>
+    <t>2092</t>
+  </si>
+  <si>
+    <t>2093</t>
+  </si>
+  <si>
+    <t>2095</t>
+  </si>
+  <si>
+    <t>2097</t>
+  </si>
+  <si>
+    <t>2098</t>
+  </si>
+  <si>
+    <t>2099</t>
+  </si>
+  <si>
+    <t>2100</t>
+  </si>
+  <si>
+    <t>2101</t>
+  </si>
+  <si>
+    <t>2102</t>
+  </si>
+  <si>
+    <t>2103</t>
+  </si>
+  <si>
+    <t>2104</t>
+  </si>
+  <si>
+    <t>2105</t>
+  </si>
+  <si>
+    <t>2106</t>
+  </si>
+  <si>
+    <t>2107</t>
+  </si>
+  <si>
+    <t>2110</t>
+  </si>
+  <si>
+    <t>2111</t>
+  </si>
+  <si>
+    <t>2112</t>
+  </si>
+  <si>
+    <t>2113</t>
+  </si>
+  <si>
+    <t>2114</t>
+  </si>
+  <si>
+    <t>2115</t>
+  </si>
+  <si>
+    <t>2116</t>
+  </si>
+  <si>
+    <t>2117</t>
+  </si>
+  <si>
+    <t>2118</t>
+  </si>
+  <si>
+    <t>2119</t>
+  </si>
+  <si>
+    <t>2120</t>
+  </si>
+  <si>
+    <t>2121</t>
+  </si>
+  <si>
+    <t>2122</t>
+  </si>
+  <si>
+    <t>2123</t>
+  </si>
+  <si>
+    <t>2124</t>
+  </si>
+  <si>
+    <t>2125</t>
+  </si>
+  <si>
+    <t>2126</t>
+  </si>
+  <si>
+    <t>2127</t>
+  </si>
+  <si>
+    <t>2128</t>
+  </si>
+  <si>
+    <t>2129</t>
+  </si>
+  <si>
+    <t>2130</t>
+  </si>
+  <si>
+    <t>2131</t>
+  </si>
+  <si>
+    <t>2132</t>
+  </si>
+  <si>
+    <t>2133</t>
+  </si>
+  <si>
+    <t>2134</t>
+  </si>
+  <si>
+    <t>2135</t>
+  </si>
+  <si>
+    <t>2136</t>
+  </si>
+  <si>
+    <t>2137</t>
+  </si>
+  <si>
+    <t>2138</t>
+  </si>
+  <si>
+    <t>2139</t>
+  </si>
+  <si>
+    <t>2140</t>
+  </si>
+  <si>
+    <t>2141</t>
+  </si>
+  <si>
+    <t>2142</t>
+  </si>
+  <si>
+    <t>2143</t>
+  </si>
+  <si>
+    <t>2144</t>
+  </si>
+  <si>
+    <t>2145</t>
+  </si>
+  <si>
+    <t>2146</t>
+  </si>
+  <si>
+    <t>2147</t>
+  </si>
+  <si>
+    <t>2148</t>
+  </si>
+  <si>
+    <t>2149</t>
+  </si>
+  <si>
+    <t>2150</t>
+  </si>
+  <si>
+    <t>2151</t>
+  </si>
+  <si>
+    <t>2153</t>
+  </si>
+  <si>
+    <t>2154</t>
+  </si>
+  <si>
+    <t>2156</t>
+  </si>
+  <si>
+    <t>2157</t>
+  </si>
+  <si>
+    <t>2158</t>
+  </si>
+  <si>
+    <t>2159</t>
+  </si>
+  <si>
+    <t>2160</t>
+  </si>
+  <si>
+    <t>2171</t>
+  </si>
+  <si>
+    <t>2172</t>
+  </si>
+  <si>
+    <t>2173</t>
+  </si>
+  <si>
+    <t>2174</t>
+  </si>
+  <si>
+    <t>2180</t>
+  </si>
+  <si>
+    <t>2181</t>
+  </si>
+  <si>
+    <t>2182</t>
+  </si>
+  <si>
+    <t>2183</t>
+  </si>
+  <si>
+    <t>2184</t>
+  </si>
+  <si>
+    <t>2185</t>
+  </si>
+  <si>
+    <t>2186</t>
+  </si>
+  <si>
+    <t>68.0</t>
+  </si>
+  <si>
+    <t>2187</t>
+  </si>
+  <si>
+    <t>2188</t>
+  </si>
+  <si>
+    <t>2189</t>
+  </si>
+  <si>
+    <t>2190</t>
+  </si>
+  <si>
+    <t>2191</t>
+  </si>
+  <si>
+    <t>2192</t>
+  </si>
+  <si>
+    <t>2193</t>
+  </si>
+  <si>
+    <t>2194</t>
+  </si>
+  <si>
+    <t>2195</t>
+  </si>
+  <si>
+    <t>2196</t>
+  </si>
+  <si>
+    <t>2197</t>
+  </si>
+  <si>
+    <t>2198</t>
+  </si>
+  <si>
+    <t>2199</t>
+  </si>
+  <si>
+    <t>2200</t>
+  </si>
+  <si>
+    <t>2201</t>
+  </si>
+  <si>
+    <t>2202</t>
+  </si>
+  <si>
+    <t>2203</t>
+  </si>
+  <si>
+    <t>2204</t>
+  </si>
+  <si>
+    <t>2205</t>
+  </si>
+  <si>
+    <t>2206</t>
+  </si>
+  <si>
+    <t>2207</t>
+  </si>
+  <si>
+    <t>2208</t>
+  </si>
+  <si>
+    <t>2209</t>
+  </si>
+  <si>
+    <t>2210</t>
+  </si>
+  <si>
+    <t>2211</t>
+  </si>
+  <si>
+    <t>2212</t>
+  </si>
+  <si>
+    <t>2213</t>
+  </si>
+  <si>
+    <t>2214</t>
+  </si>
+  <si>
+    <t>2215</t>
+  </si>
+  <si>
+    <t>2216</t>
+  </si>
+  <si>
+    <t>2217</t>
+  </si>
+  <si>
+    <t>2218</t>
+  </si>
+  <si>
+    <t>2219</t>
+  </si>
+  <si>
+    <t>2220</t>
+  </si>
+  <si>
+    <t>2221</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+  <si>
+    <t>2223</t>
+  </si>
+  <si>
+    <t>2224</t>
+  </si>
+  <si>
+    <t>2225</t>
+  </si>
+  <si>
+    <t>2226</t>
+  </si>
+  <si>
+    <t>2227</t>
+  </si>
+  <si>
+    <t>2228</t>
+  </si>
+  <si>
+    <t>2229</t>
+  </si>
+  <si>
+    <t>2230</t>
+  </si>
+  <si>
+    <t>2231</t>
+  </si>
+  <si>
+    <t>2232</t>
+  </si>
+  <si>
+    <t>2233</t>
+  </si>
+  <si>
+    <t>2234</t>
+  </si>
+  <si>
+    <t>2235</t>
+  </si>
+  <si>
+    <t>2236</t>
+  </si>
+  <si>
+    <t>2237</t>
+  </si>
+  <si>
+    <t>2238</t>
+  </si>
+  <si>
+    <t>2239</t>
+  </si>
+  <si>
+    <t>2240</t>
+  </si>
+  <si>
+    <t>2241</t>
+  </si>
+  <si>
+    <t>2242</t>
+  </si>
+  <si>
+    <t>2243</t>
+  </si>
+  <si>
+    <t>2244</t>
+  </si>
+  <si>
+    <t>2245</t>
+  </si>
+  <si>
+    <t>2246</t>
+  </si>
+  <si>
+    <t>2247</t>
+  </si>
+  <si>
+    <t>2248</t>
+  </si>
+  <si>
+    <t>2249</t>
+  </si>
+  <si>
+    <t>2250</t>
+  </si>
+  <si>
+    <t>2251</t>
+  </si>
+  <si>
+    <t>2253</t>
+  </si>
+  <si>
+    <t>2254</t>
+  </si>
+  <si>
+    <t>2255</t>
+  </si>
+  <si>
+    <t>2256</t>
+  </si>
+  <si>
+    <t>2257</t>
+  </si>
+  <si>
+    <t>203.0</t>
+  </si>
+  <si>
+    <t>11953</t>
+  </si>
+  <si>
+    <t>12459</t>
+  </si>
+  <si>
+    <t>210.0</t>
+  </si>
+  <si>
+    <t>12461</t>
+  </si>
+  <si>
+    <t>12462</t>
+  </si>
+  <si>
+    <t>12463</t>
+  </si>
+  <si>
+    <t>12464</t>
+  </si>
+  <si>
+    <t>12465</t>
+  </si>
+  <si>
+    <t>12466</t>
+  </si>
+  <si>
+    <t>12467</t>
+  </si>
+  <si>
+    <t>12468</t>
+  </si>
+  <si>
+    <t>12469</t>
+  </si>
+  <si>
+    <t>12470</t>
+  </si>
+  <si>
+    <t>12471</t>
+  </si>
+  <si>
+    <t>12472</t>
+  </si>
+  <si>
+    <t>12473</t>
+  </si>
+  <si>
+    <t>12474</t>
+  </si>
+  <si>
+    <t>12475</t>
+  </si>
+  <si>
+    <t>12476</t>
+  </si>
+  <si>
+    <t>12477</t>
+  </si>
+  <si>
+    <t>12478</t>
+  </si>
+  <si>
+    <t>12487</t>
+  </si>
+  <si>
+    <t>211.0</t>
+  </si>
+  <si>
+    <t>12488</t>
+  </si>
+  <si>
+    <t>12489</t>
+  </si>
+  <si>
+    <t>12490</t>
+  </si>
+  <si>
+    <t>12491</t>
+  </si>
+  <si>
+    <t>12492</t>
+  </si>
+  <si>
+    <t>12493</t>
+  </si>
+  <si>
+    <t>12494</t>
+  </si>
+  <si>
+    <t>12495</t>
+  </si>
+  <si>
+    <t>12496</t>
+  </si>
+  <si>
+    <t>12497</t>
+  </si>
+  <si>
+    <t>12498</t>
+  </si>
+  <si>
+    <t>12499</t>
+  </si>
+  <si>
+    <t>12500</t>
+  </si>
+  <si>
+    <t>12501</t>
+  </si>
+  <si>
+    <t>12502</t>
+  </si>
+  <si>
+    <t>12503</t>
+  </si>
+  <si>
+    <t>12504</t>
+  </si>
+  <si>
+    <t>12505</t>
+  </si>
+  <si>
+    <t>12506</t>
+  </si>
+  <si>
+    <t>12507</t>
+  </si>
+  <si>
+    <t>12508</t>
+  </si>
+  <si>
+    <t>12509</t>
+  </si>
+  <si>
+    <t>12510</t>
+  </si>
+  <si>
+    <t>12511</t>
+  </si>
+  <si>
+    <t>12512</t>
+  </si>
+  <si>
+    <t>12513</t>
+  </si>
+  <si>
+    <t>12514</t>
+  </si>
+  <si>
+    <t>12523</t>
+  </si>
+  <si>
+    <t>12524</t>
+  </si>
+  <si>
+    <t>12525</t>
+  </si>
+  <si>
+    <t>12526</t>
+  </si>
+  <si>
+    <t>12527</t>
+  </si>
+  <si>
+    <t>12528</t>
+  </si>
+  <si>
+    <t>12529</t>
+  </si>
+  <si>
+    <t>12530</t>
+  </si>
+  <si>
+    <t>12531</t>
+  </si>
+  <si>
+    <t>12532</t>
+  </si>
+  <si>
+    <t>12533</t>
+  </si>
+  <si>
+    <t>12534</t>
+  </si>
+  <si>
+    <t>12535</t>
+  </si>
+  <si>
+    <t>12536</t>
+  </si>
+  <si>
+    <t>12537</t>
+  </si>
+  <si>
+    <t>12538</t>
+  </si>
+  <si>
+    <t>12539</t>
+  </si>
+  <si>
+    <t>12540</t>
+  </si>
+  <si>
+    <t>12541</t>
+  </si>
+  <si>
+    <t>12542</t>
+  </si>
+  <si>
+    <t>12543</t>
+  </si>
+  <si>
+    <t>12544</t>
+  </si>
+  <si>
+    <t>12545</t>
+  </si>
+  <si>
+    <t>12546</t>
+  </si>
+  <si>
+    <t>12547</t>
+  </si>
+  <si>
+    <t>12583</t>
+  </si>
+  <si>
+    <t>212.0</t>
+  </si>
+  <si>
+    <t>12585</t>
+  </si>
+  <si>
+    <t>12586</t>
+  </si>
+  <si>
+    <t>12587</t>
+  </si>
+  <si>
+    <t>12588</t>
+  </si>
+  <si>
+    <t>12589</t>
+  </si>
+  <si>
+    <t>12590</t>
+  </si>
+  <si>
+    <t>12591</t>
+  </si>
+  <si>
+    <t>12592</t>
+  </si>
+  <si>
+    <t>12593</t>
+  </si>
+  <si>
+    <t>12594</t>
+  </si>
+  <si>
+    <t>12595</t>
+  </si>
+  <si>
+    <t>12596</t>
+  </si>
+  <si>
+    <t>12597</t>
+  </si>
+  <si>
+    <t>12598</t>
+  </si>
+  <si>
+    <t>12599</t>
+  </si>
+  <si>
+    <t>12600</t>
+  </si>
+  <si>
+    <t>12601</t>
+  </si>
+  <si>
+    <t>12602</t>
+  </si>
+  <si>
+    <t>12603</t>
+  </si>
+  <si>
+    <t>12604</t>
+  </si>
+  <si>
+    <t>12605</t>
+  </si>
+  <si>
+    <t>12606</t>
+  </si>
+  <si>
+    <t>12607</t>
+  </si>
+  <si>
+    <t>213.0</t>
+  </si>
+  <si>
+    <t>214.0</t>
   </si>
 </sst>
 </file>
@@ -13024,7 +14869,7 @@
         <v>6000</v>
       </c>
       <c r="D2" t="s">
-        <v>708</v>
+        <v>3040</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -13033,7 +14878,7 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>4202</v>
+        <v>4817</v>
       </c>
       <c r="H2">
         <v>25</v>

</xml_diff>